<commit_message>
modify pincode insert error
</commit_message>
<xml_diff>
--- a/Web2Pair2.xlsx
+++ b/Web2Pair2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20610" windowHeight="8250"/>
@@ -10,17 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -457,9 +447,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -764,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1358,7 @@
       <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G10" t="s">
@@ -2304,6 +2291,7 @@
   <hyperlinks>
     <hyperlink ref="F7" r:id="rId1" location="!/catalog/new?bnid=home_info_comm_pers_te85400361&amp;gem_catalog_id=5116877-14241044019"/>
     <hyperlink ref="F2" r:id="rId2" location="!/catalog/new?bnid=home_info_comm_pers_te85400361&amp;gem_catalog_id=5116877-95889357017"/>
+    <hyperlink ref="F10" r:id="rId3" location="!/catalog/new?bnid=home_info_comm_pers_te85400361&amp;gem_catalog_id=5116877-58687788922"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>